<commit_message>
Changes after testing and protection
</commit_message>
<xml_diff>
--- a/src/main/resources/static/resources/ResultSheet.xlsx
+++ b/src/main/resources/static/resources/ResultSheet.xlsx
@@ -101,7 +101,7 @@
     <t>Batting</t>
   </si>
   <si>
-    <t>Match drawn</t>
+    <t>Match tied</t>
   </si>
 </sst>
 </file>
@@ -254,17 +254,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -285,25 +281,30 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
-      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -587,7 +588,7 @@
   <dimension ref="A1:S33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="C2" sqref="C2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -602,14 +603,16 @@
     <col min="9" max="10" width="11.7109375" style="1"/>
     <col min="11" max="11" width="6.42578125" style="1" customWidth="1"/>
     <col min="12" max="13" width="11.7109375" style="1"/>
-    <col min="14" max="16" width="9.140625" style="1"/>
-    <col min="17" max="17" width="13.42578125" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="1"/>
+    <col min="14" max="15" width="9.140625" style="1"/>
+    <col min="16" max="16" width="0" style="1" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="13.42578125" style="1" hidden="1" customWidth="1"/>
+    <col min="18" max="19" width="0" style="1" hidden="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="17.25" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="12"/>
-      <c r="B1" s="13" t="s">
+      <c r="A1" s="11"/>
+      <c r="B1" s="12" t="s">
         <v>22</v>
       </c>
     </row>
@@ -617,16 +620,16 @@
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="23"/>
       <c r="E2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="23"/>
       <c r="K2" s="2" t="s">
         <v>1</v>
       </c>
@@ -648,18 +651,18 @@
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="H3" s="15" t="s">
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="H3" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
       <c r="P3" s="1" t="b">
         <f>NOT(ISBLANK(I2))</f>
         <v>0</v>
@@ -683,7 +686,7 @@
         <v>0</v>
       </c>
       <c r="Q4" s="1">
-        <f>ABS(Q2-Q3)</f>
+        <f>Q2-Q3</f>
         <v>0</v>
       </c>
     </row>
@@ -734,7 +737,7 @@
         <v>7</v>
       </c>
       <c r="P6" s="1" t="b">
-        <f>AND(P5,Q4&gt;0)</f>
+        <f>AND(P4,Q4&gt;0)</f>
         <v>0</v>
       </c>
       <c r="Q6" s="1" t="str">
@@ -752,23 +755,23 @@
       <c r="A7" s="4">
         <v>1</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="6"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="5"/>
       <c r="G7" s="4">
         <v>1</v>
       </c>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="6"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="5"/>
       <c r="P7" s="1" t="b">
         <f>AND(P4,Q4&lt;0)</f>
         <v>0</v>
       </c>
       <c r="Q7" s="1" t="str">
-        <f>I23&amp;" won by "&amp;S3&amp;" wicket"&amp;IF(S3&gt;1,"s","")</f>
+        <f>I2&amp;" won by "&amp;S3&amp;" wicket"&amp;IF(S3&gt;1,"s","")</f>
         <v xml:space="preserve"> won by 6 wickets</v>
       </c>
       <c r="R7" s="1">
@@ -782,21 +785,21 @@
       <c r="A8" s="4">
         <v>2</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="6"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="5"/>
       <c r="G8" s="4">
         <v>2</v>
       </c>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="6"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="5"/>
       <c r="P8" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="Q8" s="21" t="str">
+      <c r="Q8" s="14" t="str">
         <f>""</f>
         <v/>
       </c>
@@ -811,17 +814,17 @@
       <c r="A9" s="4">
         <v>3</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="6"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="5"/>
       <c r="G9" s="4">
         <v>3</v>
       </c>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="6"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="5"/>
       <c r="P9" s="1" t="str">
         <f>VLOOKUP(TRUE,results,2, FALSE)</f>
         <v/>
@@ -831,72 +834,72 @@
       <c r="A10" s="4">
         <v>4</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="6"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="5"/>
       <c r="G10" s="4">
         <v>4</v>
       </c>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="6"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="5"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>5</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="6"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="5"/>
       <c r="G11" s="4">
         <v>5</v>
       </c>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="6"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="5"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>6</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="6"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="5"/>
       <c r="G12" s="4">
         <v>6</v>
       </c>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="6"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="5"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="6"/>
-      <c r="J13" s="7" t="s">
+      <c r="E13" s="5"/>
+      <c r="J13" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="K13" s="6"/>
+      <c r="K13" s="5"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D14" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="8">
+      <c r="E14" s="7">
         <f>SUM(E7:E13)</f>
         <v>0</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K14" s="8">
+      <c r="K14" s="7">
         <f>SUM(K7:K13)</f>
         <v>0</v>
       </c>
@@ -905,7 +908,7 @@
       <c r="D15" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E15" s="6"/>
+      <c r="E15" s="5"/>
       <c r="F15" s="2" t="s">
         <v>10</v>
       </c>
@@ -913,7 +916,7 @@
       <c r="J15" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K15" s="6"/>
+      <c r="K15" s="5"/>
       <c r="L15" s="2" t="s">
         <v>10</v>
       </c>
@@ -927,7 +930,7 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C17" s="4" t="s">
@@ -956,125 +959,125 @@
       <c r="A18" s="4">
         <v>1</v>
       </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="6"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="5"/>
       <c r="G18" s="4">
         <v>1</v>
       </c>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="6"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="5"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>2</v>
       </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="6"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="5"/>
       <c r="G19" s="4">
         <v>2</v>
       </c>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="6"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="5"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>3</v>
       </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="6"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="5"/>
       <c r="G20" s="4">
         <v>3</v>
       </c>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="6"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="5"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>4</v>
       </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="6"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="5"/>
       <c r="G21" s="4">
         <v>4</v>
       </c>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="6"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="5"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>5</v>
       </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="6"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="5"/>
       <c r="G22" s="4">
         <v>5</v>
       </c>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="6"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="5"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>6</v>
       </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="6"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="5"/>
       <c r="G23" s="4">
         <v>6</v>
       </c>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="6"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="5"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="18" t="str">
+      <c r="C25" s="19" t="str">
         <f>P9</f>
         <v/>
       </c>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="19"/>
-      <c r="J25" s="19"/>
-      <c r="K25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="21"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B26" s="10"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="10"/>
-      <c r="H26" s="10"/>
-      <c r="I26" s="10"/>
-      <c r="J26" s="10"/>
-      <c r="K26" s="10"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="9"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H27" s="4" t="s">
@@ -1094,23 +1097,23 @@
       <c r="B28" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C28" s="16" t="str">
+      <c r="C28" s="17" t="str">
         <f>IF(P2,C2,"")</f>
         <v/>
       </c>
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="22"/>
-      <c r="G28" s="22"/>
-      <c r="H28" s="17">
-        <f>VLOOKUP(TRUE,results,3)</f>
-        <v>0</v>
-      </c>
-      <c r="I28" s="17">
+      <c r="D28" s="17"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="16">
+        <f>VLOOKUP(TRUE,results,3, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="I28" s="16">
         <f>MIN(6,MAX(0,INT((E14-60)/10)))</f>
         <v>0</v>
       </c>
-      <c r="J28" s="17">
+      <c r="J28" s="16">
         <f>K15</f>
         <v>0</v>
       </c>
@@ -1123,23 +1126,23 @@
       <c r="B29" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C29" s="16" t="str">
+      <c r="C29" s="17" t="str">
         <f>IF(P3,I2,"")</f>
         <v/>
       </c>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="22"/>
-      <c r="G29" s="22"/>
-      <c r="H29" s="17">
-        <f>VLOOKUP(TRUE,results,4)</f>
-        <v>0</v>
-      </c>
-      <c r="I29" s="17">
+      <c r="D29" s="17"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="16">
+        <f>VLOOKUP(TRUE,results,4, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="I29" s="16">
         <f>MIN(6,MAX(0,INT((E15-60)/10))+IF(P7,S3,0))</f>
         <v>0</v>
       </c>
-      <c r="J29" s="17">
+      <c r="J29" s="16">
         <f>E15</f>
         <v>0</v>
       </c>
@@ -1164,6 +1167,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="7">
     <mergeCell ref="C29:E29"/>
     <mergeCell ref="C2:D2"/>

</xml_diff>